<commit_message>
añadidos los posibles movimientos de los pokemns al excel
</commit_message>
<xml_diff>
--- a/ST/src/principal/Lista de tipos y movimientos de pokémon.xlsx
+++ b/ST/src/principal/Lista de tipos y movimientos de pokémon.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdiaz\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D802CF-1239-4286-AA47-E770540A013B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{34424F4C-CD1E-47D1-AFE5-31FDC56CF9BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13956" yWindow="5364" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="17360" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="231">
   <si>
     <t>PLANTA</t>
   </si>
@@ -427,6 +423,297 @@
   </si>
   <si>
     <t>ESPACIO RARO (?)/VENDETTA</t>
+  </si>
+  <si>
+    <t>LLAMARADA</t>
+  </si>
+  <si>
+    <t>PULSO UMBRIO</t>
+  </si>
+  <si>
+    <t>DIA SOLEADO</t>
+  </si>
+  <si>
+    <t>VUELO</t>
+  </si>
+  <si>
+    <t>ATAQUE ALA</t>
+  </si>
+  <si>
+    <t>CUCHILLADA</t>
+  </si>
+  <si>
+    <t>GOLPE CABEZA</t>
+  </si>
+  <si>
+    <t>EVITE IGNEO</t>
+  </si>
+  <si>
+    <t>PUAS TOXICAS</t>
+  </si>
+  <si>
+    <t>HIDORBOMBA</t>
+  </si>
+  <si>
+    <t>DANZA DRAGÓN</t>
+  </si>
+  <si>
+    <t>COMETA DRAGÓN</t>
+  </si>
+  <si>
+    <t>ELECTROCAÑÓN</t>
+  </si>
+  <si>
+    <t>RUGIDO</t>
+  </si>
+  <si>
+    <t>BRILLO MAGICO</t>
+  </si>
+  <si>
+    <t>PANTALLA LUZ</t>
+  </si>
+  <si>
+    <t>REFEJO</t>
+  </si>
+  <si>
+    <t>HIDROBOMBA</t>
+  </si>
+  <si>
+    <t>AQUA JET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GARRA DRAGÓN </t>
+  </si>
+  <si>
+    <t>TUMBA ROCAS</t>
+  </si>
+  <si>
+    <t>LLANZALLAMAS</t>
+  </si>
+  <si>
+    <t>COMETA DRACO</t>
+  </si>
+  <si>
+    <t>MISMO DESTINO</t>
+  </si>
+  <si>
+    <t>A BOCAJARRO</t>
+  </si>
+  <si>
+    <t>TAJO UMBRIO</t>
+  </si>
+  <si>
+    <t>PSICO CORTE</t>
+  </si>
+  <si>
+    <t>DEMOLICIÓN</t>
+  </si>
+  <si>
+    <t>AVALNACHA</t>
+  </si>
+  <si>
+    <t>CHUPAVIDAS</t>
+  </si>
+  <si>
+    <t>TIJERA X</t>
+  </si>
+  <si>
+    <t>VOLTIOCAMBIO</t>
+  </si>
+  <si>
+    <t>CARRA DRAGÓN</t>
+  </si>
+  <si>
+    <t>COLMILLO IGNEO</t>
+  </si>
+  <si>
+    <t>FUERZA LUNAR</t>
+  </si>
+  <si>
+    <t>DESEO</t>
+  </si>
+  <si>
+    <t>COME SUEÑOS</t>
+  </si>
+  <si>
+    <t>PERMONICIÓN</t>
+  </si>
+  <si>
+    <t>BOMBA LODO</t>
+  </si>
+  <si>
+    <t>GRANIZO</t>
+  </si>
+  <si>
+    <t>MORDISCO</t>
+  </si>
+  <si>
+    <t>SUSTITUTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOLPE AEREO </t>
+  </si>
+  <si>
+    <t>RESPIRO</t>
+  </si>
+  <si>
+    <t>ACROBATA</t>
+  </si>
+  <si>
+    <t>GIGADRENADO</t>
+  </si>
+  <si>
+    <t>SINTESIS</t>
+  </si>
+  <si>
+    <t>RAYO SOLAR</t>
+  </si>
+  <si>
+    <t>DOBLE PATADA</t>
+  </si>
+  <si>
+    <t>COLMILLO RAYO</t>
+  </si>
+  <si>
+    <t>VELOCIDAD EXTREMA</t>
+  </si>
+  <si>
+    <t>ATAQUE OSEO</t>
+  </si>
+  <si>
+    <t>VIENTO PLATA</t>
+  </si>
+  <si>
+    <t>ESCALDAR</t>
+  </si>
+  <si>
+    <t>IDA Y VUELTA</t>
+  </si>
+  <si>
+    <t>CONTENEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRITURAR </t>
+  </si>
+  <si>
+    <t>CORPULENCIA</t>
+  </si>
+  <si>
+    <t>TREPARROCAS</t>
+  </si>
+  <si>
+    <t>SUPERSONICO</t>
+  </si>
+  <si>
+    <t>GIRO BOLA</t>
+  </si>
+  <si>
+    <t>EXPLOXIÓN</t>
+  </si>
+  <si>
+    <t>CABEZAZO ZEN</t>
+  </si>
+  <si>
+    <t>PUÑO METEORO</t>
+  </si>
+  <si>
+    <t>AGILIDAD</t>
+  </si>
+  <si>
+    <t>RECUPERACIÓN</t>
+  </si>
+  <si>
+    <t>COLA DRAGON</t>
+  </si>
+  <si>
+    <t>TERRATEMBLOR</t>
+  </si>
+  <si>
+    <t>GARRA UMBRIA</t>
+  </si>
+  <si>
+    <t>BRILLO MÁGICO</t>
+  </si>
+  <si>
+    <t>GOLPE AEREO</t>
+  </si>
+  <si>
+    <t>TRIATAQUE</t>
+  </si>
+  <si>
+    <t>DOBLE RAYO</t>
+  </si>
+  <si>
+    <t>PSICOCARGA</t>
+  </si>
+  <si>
+    <t>PUÑO MAREO</t>
+  </si>
+  <si>
+    <t>ESPACIO RARO</t>
+  </si>
+  <si>
+    <t>TAMPA VENENOSA</t>
+  </si>
+  <si>
+    <t>ONDA TÓXICA</t>
+  </si>
+  <si>
+    <t>PODER OCULTO</t>
+  </si>
+  <si>
+    <t>LLUEVE HOJAS</t>
+  </si>
+  <si>
+    <t>DRENADORAS</t>
+  </si>
+  <si>
+    <t>GIRO VIL</t>
+  </si>
+  <si>
+    <t>MEGACUERNO</t>
+  </si>
+  <si>
+    <t>TRAMPA VENENOSA</t>
+  </si>
+  <si>
+    <t>GOLPE BAJO</t>
+  </si>
+  <si>
+    <t>BESO DRENAJE</t>
+  </si>
+  <si>
+    <t>PAN MENTAL</t>
+  </si>
+  <si>
+    <t>RAPIDEZ</t>
+  </si>
+  <si>
+    <t>HUMREDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROTECCIÓN </t>
+  </si>
+  <si>
+    <t>TAJO AEREO</t>
+  </si>
+  <si>
+    <t>ESFERA AURAL</t>
+  </si>
+  <si>
+    <t>ARMADURA ACIDA</t>
+  </si>
+  <si>
+    <t>SOMNIFERO</t>
+  </si>
+  <si>
+    <t>DANZA PETALO</t>
+  </si>
+  <si>
+    <t>CARATOÑA</t>
+  </si>
+  <si>
+    <t>ALA DE ACERO</t>
   </si>
 </sst>
 </file>
@@ -746,13 +1033,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" customWidth="1"/>
+    <col min="6" max="6" width="29.36328125" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" customWidth="1"/>
+    <col min="8" max="8" width="20.26953125" customWidth="1"/>
+    <col min="9" max="9" width="16.1796875" customWidth="1"/>
+    <col min="10" max="10" width="18.90625" customWidth="1"/>
+    <col min="11" max="11" width="24" customWidth="1"/>
+    <col min="12" max="12" width="15.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>18</v>
       </c>
@@ -760,7 +1060,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -771,7 +1071,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -782,7 +1082,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -793,7 +1093,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -804,7 +1104,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -815,7 +1115,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -826,7 +1126,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -837,7 +1137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -848,7 +1148,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -859,7 +1159,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -870,7 +1170,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -881,7 +1181,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -892,7 +1192,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -903,7 +1203,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -914,7 +1214,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -925,7 +1225,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -936,7 +1236,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -947,7 +1247,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -958,57 +1258,57 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="L32">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -1043,7 +1343,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -1078,7 +1378,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1113,7 +1413,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1148,7 +1448,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -1183,7 +1483,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -1218,7 +1518,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -1253,224 +1553,1544 @@
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" t="s">
+        <v>26</v>
+      </c>
+      <c r="H40" t="s">
+        <v>132</v>
+      </c>
+      <c r="I40" t="s">
+        <v>135</v>
+      </c>
+      <c r="J40" t="s">
+        <v>33</v>
+      </c>
+      <c r="K40" t="s">
+        <v>136</v>
+      </c>
+      <c r="L40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" t="s">
+        <v>138</v>
+      </c>
+      <c r="E41" t="s">
+        <v>134</v>
+      </c>
+      <c r="F41" t="s">
+        <v>36</v>
+      </c>
+      <c r="G41" t="s">
+        <v>139</v>
+      </c>
+      <c r="H41" t="s">
+        <v>33</v>
+      </c>
+      <c r="I41" t="s">
+        <v>122</v>
+      </c>
+      <c r="J41" t="s">
+        <v>140</v>
+      </c>
+      <c r="K41" t="s">
+        <v>121</v>
+      </c>
+      <c r="L41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>142</v>
+      </c>
+      <c r="D42" t="s">
+        <v>143</v>
+      </c>
+      <c r="E42" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" t="s">
+        <v>49</v>
+      </c>
+      <c r="G42" t="s">
+        <v>43</v>
+      </c>
+      <c r="H42" t="s">
+        <v>33</v>
+      </c>
+      <c r="I42" t="s">
+        <v>30</v>
+      </c>
+      <c r="J42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K42" t="s">
+        <v>129</v>
+      </c>
+      <c r="L42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" t="s">
+        <v>138</v>
+      </c>
+      <c r="E43" t="s">
+        <v>137</v>
+      </c>
+      <c r="F43" t="s">
+        <v>41</v>
+      </c>
+      <c r="G43" t="s">
+        <v>145</v>
+      </c>
+      <c r="H43" t="s">
+        <v>37</v>
+      </c>
+      <c r="I43" t="s">
+        <v>30</v>
+      </c>
+      <c r="J43" t="s">
+        <v>42</v>
+      </c>
+      <c r="K43" t="s">
+        <v>33</v>
+      </c>
+      <c r="L43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" t="s">
+        <v>146</v>
+      </c>
+      <c r="E44" t="s">
+        <v>140</v>
+      </c>
+      <c r="F44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" t="s">
+        <v>47</v>
+      </c>
+      <c r="H44" t="s">
+        <v>33</v>
+      </c>
+      <c r="I44" t="s">
+        <v>41</v>
+      </c>
+      <c r="J44" t="s">
+        <v>33</v>
+      </c>
+      <c r="K44" t="s">
+        <v>147</v>
+      </c>
+      <c r="L44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" t="s">
+        <v>132</v>
+      </c>
+      <c r="E45" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" t="s">
+        <v>30</v>
+      </c>
+      <c r="G45" t="s">
+        <v>26</v>
+      </c>
+      <c r="H45" t="s">
+        <v>148</v>
+      </c>
+      <c r="I45" t="s">
+        <v>150</v>
+      </c>
+      <c r="J45" t="s">
+        <v>42</v>
+      </c>
+      <c r="K45" t="s">
+        <v>149</v>
+      </c>
+      <c r="L45" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>151</v>
+      </c>
+      <c r="D46" t="s">
+        <v>152</v>
+      </c>
+      <c r="E46" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" t="s">
+        <v>49</v>
+      </c>
+      <c r="H46" t="s">
+        <v>24</v>
+      </c>
+      <c r="I46" t="s">
+        <v>43</v>
+      </c>
+      <c r="J46" t="s">
+        <v>42</v>
+      </c>
+      <c r="K46" t="s">
+        <v>129</v>
+      </c>
+      <c r="L46" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" t="s">
+        <v>45</v>
+      </c>
+      <c r="E47" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" t="s">
+        <v>155</v>
+      </c>
+      <c r="H47" t="s">
+        <v>156</v>
+      </c>
+      <c r="I47" t="s">
+        <v>137</v>
+      </c>
+      <c r="J47" t="s">
+        <v>42</v>
+      </c>
+      <c r="K47" t="s">
+        <v>34</v>
+      </c>
+      <c r="L47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" t="s">
+        <v>157</v>
+      </c>
+      <c r="F48" t="s">
+        <v>131</v>
+      </c>
+      <c r="G48" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" t="s">
+        <v>41</v>
+      </c>
+      <c r="I48" t="s">
+        <v>32</v>
+      </c>
+      <c r="J48" t="s">
+        <v>30</v>
+      </c>
+      <c r="K48" t="s">
+        <v>33</v>
+      </c>
+      <c r="L48" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>158</v>
+      </c>
+      <c r="D49" t="s">
+        <v>139</v>
+      </c>
+      <c r="E49" t="s">
+        <v>159</v>
+      </c>
+      <c r="F49" t="s">
+        <v>160</v>
+      </c>
+      <c r="G49" t="s">
+        <v>132</v>
+      </c>
+      <c r="H49" t="s">
+        <v>33</v>
+      </c>
+      <c r="I49" t="s">
+        <v>9</v>
+      </c>
+      <c r="J49" t="s">
+        <v>148</v>
+      </c>
+      <c r="K49" t="s">
+        <v>161</v>
+      </c>
+      <c r="L49" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" t="s">
+        <v>41</v>
+      </c>
+      <c r="E50" t="s">
+        <v>139</v>
+      </c>
+      <c r="F50" t="s">
+        <v>163</v>
+      </c>
+      <c r="G50" t="s">
+        <v>164</v>
+      </c>
+      <c r="H50" t="s">
+        <v>33</v>
+      </c>
+      <c r="I50" t="s">
+        <v>30</v>
+      </c>
+      <c r="J50" t="s">
+        <v>29</v>
+      </c>
+      <c r="K50" t="s">
+        <v>165</v>
+      </c>
+      <c r="L50" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>166</v>
+      </c>
+      <c r="D51" t="s">
+        <v>45</v>
+      </c>
+      <c r="E51" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" t="s">
+        <v>167</v>
+      </c>
+      <c r="G51" t="s">
+        <v>46</v>
+      </c>
+      <c r="H51" t="s">
+        <v>156</v>
+      </c>
+      <c r="I51" t="s">
+        <v>30</v>
+      </c>
+      <c r="J51" t="s">
+        <v>121</v>
+      </c>
+      <c r="K51" t="s">
+        <v>35</v>
+      </c>
+      <c r="L51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>168</v>
+      </c>
+      <c r="D52" t="s">
+        <v>132</v>
+      </c>
+      <c r="E52" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" t="s">
+        <v>130</v>
+      </c>
+      <c r="G52" t="s">
+        <v>169</v>
+      </c>
+      <c r="H52" t="s">
+        <v>33</v>
+      </c>
+      <c r="I52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J52" t="s">
+        <v>28</v>
+      </c>
+      <c r="K52" t="s">
+        <v>170</v>
+      </c>
+      <c r="L52" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" t="s">
+        <v>135</v>
+      </c>
+      <c r="F53" t="s">
+        <v>157</v>
+      </c>
+      <c r="G53" t="s">
+        <v>130</v>
+      </c>
+      <c r="H53" t="s">
+        <v>33</v>
+      </c>
+      <c r="I53" t="s">
+        <v>127</v>
+      </c>
+      <c r="J53" t="s">
+        <v>148</v>
+      </c>
+      <c r="K53" t="s">
+        <v>172</v>
+      </c>
+      <c r="L53" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D54" t="s">
+        <v>173</v>
+      </c>
+      <c r="E54" t="s">
+        <v>116</v>
+      </c>
+      <c r="F54" t="s">
+        <v>43</v>
+      </c>
+      <c r="G54" t="s">
+        <v>174</v>
+      </c>
+      <c r="H54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I54" t="s">
+        <v>33</v>
+      </c>
+      <c r="J54" t="s">
+        <v>28</v>
+      </c>
+      <c r="K54" t="s">
+        <v>30</v>
+      </c>
+      <c r="L54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>176</v>
+      </c>
+      <c r="D55" t="s">
+        <v>177</v>
+      </c>
+      <c r="E55" t="s">
+        <v>135</v>
+      </c>
+      <c r="F55" t="s">
+        <v>121</v>
+      </c>
+      <c r="G55" t="s">
+        <v>172</v>
+      </c>
+      <c r="H55" t="s">
+        <v>33</v>
+      </c>
+      <c r="I55" t="s">
+        <v>45</v>
+      </c>
+      <c r="J55" t="s">
+        <v>35</v>
+      </c>
+      <c r="K55" t="s">
+        <v>178</v>
+      </c>
+      <c r="L55" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>179</v>
+      </c>
+      <c r="D56" t="s">
+        <v>121</v>
+      </c>
+      <c r="E56" t="s">
+        <v>180</v>
+      </c>
+      <c r="F56" t="s">
+        <v>30</v>
+      </c>
+      <c r="G56" t="s">
+        <v>28</v>
+      </c>
+      <c r="H56" t="s">
+        <v>33</v>
+      </c>
+      <c r="I56" t="s">
+        <v>164</v>
+      </c>
+      <c r="J56" t="s">
+        <v>181</v>
+      </c>
+      <c r="K56" t="s">
+        <v>29</v>
+      </c>
+      <c r="L56" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" t="s">
+        <v>41</v>
+      </c>
+      <c r="E57" t="s">
+        <v>33</v>
+      </c>
+      <c r="F57" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" t="s">
+        <v>28</v>
+      </c>
+      <c r="H57" t="s">
+        <v>182</v>
+      </c>
+      <c r="I57" t="s">
+        <v>183</v>
+      </c>
+      <c r="J57" t="s">
+        <v>140</v>
+      </c>
+      <c r="K57" t="s">
+        <v>165</v>
+      </c>
+      <c r="L57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>158</v>
+      </c>
+      <c r="D58" t="s">
+        <v>121</v>
+      </c>
+      <c r="E58" t="s">
+        <v>184</v>
+      </c>
+      <c r="F58" t="s">
+        <v>185</v>
+      </c>
+      <c r="G58" t="s">
+        <v>30</v>
+      </c>
+      <c r="H58" t="s">
+        <v>33</v>
+      </c>
+      <c r="I58" t="s">
+        <v>28</v>
+      </c>
+      <c r="J58" t="s">
+        <v>35</v>
+      </c>
+      <c r="K58" t="s">
+        <v>45</v>
+      </c>
+      <c r="L58" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" t="s">
+        <v>129</v>
+      </c>
+      <c r="E59" t="s">
+        <v>186</v>
+      </c>
+      <c r="F59" t="s">
+        <v>24</v>
+      </c>
+      <c r="G59" t="s">
+        <v>187</v>
+      </c>
+      <c r="H59" t="s">
+        <v>188</v>
+      </c>
+      <c r="I59" t="s">
+        <v>42</v>
+      </c>
+      <c r="J59" t="s">
+        <v>33</v>
+      </c>
+      <c r="K59" t="s">
+        <v>30</v>
+      </c>
+      <c r="L59" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60" t="s">
+        <v>183</v>
+      </c>
+      <c r="E60" t="s">
+        <v>44</v>
+      </c>
+      <c r="F60" t="s">
+        <v>41</v>
+      </c>
+      <c r="G60" t="s">
+        <v>30</v>
+      </c>
+      <c r="H60" t="s">
+        <v>33</v>
+      </c>
+      <c r="I60" t="s">
+        <v>147</v>
+      </c>
+      <c r="J60" t="s">
+        <v>189</v>
+      </c>
+      <c r="K60" t="s">
+        <v>165</v>
+      </c>
+      <c r="L60" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61" t="s">
+        <v>190</v>
+      </c>
+      <c r="E61" t="s">
+        <v>46</v>
+      </c>
+      <c r="F61" t="s">
+        <v>191</v>
+      </c>
+      <c r="G61" t="s">
+        <v>161</v>
+      </c>
+      <c r="H61" t="s">
+        <v>30</v>
+      </c>
+      <c r="I61" t="s">
+        <v>33</v>
+      </c>
+      <c r="J61" t="s">
+        <v>154</v>
+      </c>
+      <c r="K61" t="s">
+        <v>121</v>
+      </c>
+      <c r="L61" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>47</v>
+      </c>
+      <c r="D62" t="s">
+        <v>40</v>
+      </c>
+      <c r="E62" t="s">
+        <v>41</v>
+      </c>
+      <c r="F62" t="s">
+        <v>193</v>
+      </c>
+      <c r="G62" t="s">
+        <v>194</v>
+      </c>
+      <c r="H62" t="s">
+        <v>30</v>
+      </c>
+      <c r="I62" t="s">
+        <v>33</v>
+      </c>
+      <c r="J62" t="s">
+        <v>108</v>
+      </c>
+      <c r="K62" t="s">
+        <v>165</v>
+      </c>
+      <c r="L62" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" t="s">
+        <v>119</v>
+      </c>
+      <c r="E63" t="s">
+        <v>196</v>
+      </c>
+      <c r="F63" t="s">
+        <v>197</v>
+      </c>
+      <c r="G63" t="s">
+        <v>45</v>
+      </c>
+      <c r="H63" t="s">
+        <v>46</v>
+      </c>
+      <c r="I63" t="s">
+        <v>172</v>
+      </c>
+      <c r="J63" t="s">
+        <v>194</v>
+      </c>
+      <c r="K63" t="s">
+        <v>198</v>
+      </c>
+      <c r="L63" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>49</v>
+      </c>
+      <c r="D64" t="s">
+        <v>24</v>
+      </c>
+      <c r="E64" t="s">
+        <v>129</v>
+      </c>
+      <c r="F64" t="s">
+        <v>199</v>
+      </c>
+      <c r="G64" t="s">
+        <v>200</v>
+      </c>
+      <c r="H64" t="s">
+        <v>43</v>
+      </c>
+      <c r="I64" t="s">
+        <v>30</v>
+      </c>
+      <c r="J64" t="s">
+        <v>201</v>
+      </c>
+      <c r="K64" t="s">
+        <v>187</v>
+      </c>
+      <c r="L64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>168</v>
+      </c>
+      <c r="D65" t="s">
+        <v>202</v>
+      </c>
+      <c r="E65" t="s">
+        <v>139</v>
+      </c>
+      <c r="F65" t="s">
+        <v>103</v>
+      </c>
+      <c r="G65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H65" t="s">
+        <v>164</v>
+      </c>
+      <c r="I65" t="s">
+        <v>9</v>
+      </c>
+      <c r="J65" t="s">
+        <v>33</v>
+      </c>
+      <c r="K65" t="s">
+        <v>203</v>
+      </c>
+      <c r="L65" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>132</v>
+      </c>
+      <c r="D66" t="s">
+        <v>26</v>
+      </c>
+      <c r="E66" t="s">
+        <v>203</v>
+      </c>
+      <c r="F66" t="s">
+        <v>135</v>
+      </c>
+      <c r="G66" t="s">
+        <v>41</v>
+      </c>
+      <c r="H66" t="s">
+        <v>28</v>
+      </c>
+      <c r="I66" t="s">
+        <v>204</v>
+      </c>
+      <c r="J66" t="s">
+        <v>29</v>
+      </c>
+      <c r="K66" t="s">
+        <v>30</v>
+      </c>
+      <c r="L66" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>205</v>
+      </c>
+      <c r="D67" t="s">
+        <v>146</v>
+      </c>
+      <c r="E67" t="s">
+        <v>199</v>
+      </c>
+      <c r="F67" t="s">
+        <v>206</v>
+      </c>
+      <c r="G67" t="s">
+        <v>41</v>
+      </c>
+      <c r="H67" t="s">
+        <v>207</v>
+      </c>
+      <c r="I67" t="s">
+        <v>198</v>
+      </c>
+      <c r="J67" t="s">
+        <v>204</v>
+      </c>
+      <c r="K67" t="s">
+        <v>30</v>
+      </c>
+      <c r="L67" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E68" t="s">
+        <v>132</v>
+      </c>
+      <c r="F68" t="s">
+        <v>33</v>
+      </c>
+      <c r="G68" t="s">
+        <v>161</v>
+      </c>
+      <c r="H68" t="s">
+        <v>207</v>
+      </c>
+      <c r="I68" t="s">
+        <v>47</v>
+      </c>
+      <c r="J68" t="s">
+        <v>30</v>
+      </c>
+      <c r="K68" t="s">
+        <v>165</v>
+      </c>
+      <c r="L68" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>208</v>
+      </c>
+      <c r="D69" t="s">
+        <v>132</v>
+      </c>
+      <c r="E69" t="s">
+        <v>28</v>
+      </c>
+      <c r="F69" t="s">
+        <v>29</v>
+      </c>
+      <c r="G69" t="s">
+        <v>209</v>
+      </c>
+      <c r="H69" t="s">
+        <v>207</v>
+      </c>
+      <c r="I69" t="s">
+        <v>33</v>
+      </c>
+      <c r="J69" t="s">
+        <v>9</v>
+      </c>
+      <c r="K69" t="s">
+        <v>194</v>
+      </c>
+      <c r="L69" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D70" t="s">
+        <v>172</v>
+      </c>
+      <c r="E70" t="s">
+        <v>30</v>
+      </c>
+      <c r="F70" t="s">
+        <v>210</v>
+      </c>
+      <c r="G70" t="s">
+        <v>127</v>
+      </c>
+      <c r="H70" t="s">
+        <v>31</v>
+      </c>
+      <c r="I70" t="s">
+        <v>33</v>
+      </c>
+      <c r="J70" t="s">
+        <v>189</v>
+      </c>
+      <c r="K70" t="s">
+        <v>211</v>
+      </c>
+      <c r="L70" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>179</v>
+      </c>
+      <c r="D71" t="s">
+        <v>164</v>
+      </c>
+      <c r="E71" t="s">
+        <v>180</v>
+      </c>
+      <c r="F71" t="s">
+        <v>213</v>
+      </c>
+      <c r="G71" t="s">
+        <v>159</v>
+      </c>
+      <c r="H71" t="s">
+        <v>36</v>
+      </c>
+      <c r="I71" t="s">
+        <v>45</v>
+      </c>
+      <c r="J71" t="s">
+        <v>154</v>
+      </c>
+      <c r="K71" t="s">
+        <v>30</v>
+      </c>
+      <c r="L71" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>216</v>
+      </c>
+      <c r="D72" t="s">
+        <v>172</v>
+      </c>
+      <c r="E72" t="s">
+        <v>127</v>
+      </c>
+      <c r="F72" t="s">
+        <v>164</v>
+      </c>
+      <c r="G72" t="s">
+        <v>217</v>
+      </c>
+      <c r="H72" t="s">
+        <v>30</v>
+      </c>
+      <c r="I72" t="s">
+        <v>194</v>
+      </c>
+      <c r="J72" t="s">
+        <v>45</v>
+      </c>
+      <c r="K72" t="s">
+        <v>33</v>
+      </c>
+      <c r="L72" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
+        <v>179</v>
+      </c>
+      <c r="D73" t="s">
+        <v>132</v>
+      </c>
+      <c r="E73" t="s">
+        <v>29</v>
+      </c>
+      <c r="F73" t="s">
+        <v>214</v>
+      </c>
+      <c r="G73" t="s">
+        <v>200</v>
+      </c>
+      <c r="H73" t="s">
+        <v>30</v>
+      </c>
+      <c r="I73" t="s">
+        <v>215</v>
+      </c>
+      <c r="J73" t="s">
+        <v>33</v>
+      </c>
+      <c r="K73" t="s">
+        <v>181</v>
+      </c>
+      <c r="L73" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>28</v>
+      </c>
+      <c r="D74" t="s">
+        <v>131</v>
+      </c>
+      <c r="E74" t="s">
+        <v>103</v>
+      </c>
+      <c r="F74" t="s">
+        <v>218</v>
+      </c>
+      <c r="G74" t="s">
+        <v>135</v>
+      </c>
+      <c r="H74" t="s">
+        <v>132</v>
+      </c>
+      <c r="I74" t="s">
+        <v>30</v>
+      </c>
+      <c r="J74" t="s">
+        <v>9</v>
+      </c>
+      <c r="K74" t="s">
+        <v>154</v>
+      </c>
+      <c r="L74" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
+        <v>168</v>
+      </c>
+      <c r="D75" t="s">
+        <v>219</v>
+      </c>
+      <c r="E75" t="s">
+        <v>220</v>
+      </c>
+      <c r="F75" t="s">
+        <v>28</v>
+      </c>
+      <c r="G75" t="s">
+        <v>203</v>
+      </c>
+      <c r="H75" t="s">
+        <v>207</v>
+      </c>
+      <c r="I75" t="s">
+        <v>30</v>
+      </c>
+      <c r="J75" t="s">
+        <v>221</v>
+      </c>
+      <c r="K75" t="s">
+        <v>33</v>
+      </c>
+      <c r="L75" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>224</v>
+      </c>
+      <c r="D76" t="s">
+        <v>225</v>
+      </c>
+      <c r="E76" t="s">
+        <v>26</v>
+      </c>
+      <c r="F76" t="s">
+        <v>28</v>
+      </c>
+      <c r="G76" t="s">
+        <v>203</v>
+      </c>
+      <c r="H76" t="s">
+        <v>207</v>
+      </c>
+      <c r="I76" t="s">
+        <v>137</v>
+      </c>
+      <c r="J76" t="s">
+        <v>41</v>
+      </c>
+      <c r="K76" t="s">
+        <v>184</v>
+      </c>
+      <c r="L76" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>134</v>
+      </c>
+      <c r="D77" t="s">
+        <v>45</v>
+      </c>
+      <c r="E77" t="s">
+        <v>222</v>
+      </c>
+      <c r="F77" t="s">
+        <v>112</v>
+      </c>
+      <c r="G77" t="s">
+        <v>154</v>
+      </c>
+      <c r="H77" t="s">
+        <v>161</v>
+      </c>
+      <c r="I77" t="s">
+        <v>223</v>
+      </c>
+      <c r="J77" t="s">
+        <v>30</v>
+      </c>
+      <c r="K77" t="s">
+        <v>34</v>
+      </c>
+      <c r="L77" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>44</v>
+      </c>
+      <c r="D78" t="s">
+        <v>45</v>
+      </c>
+      <c r="E78" t="s">
+        <v>135</v>
+      </c>
+      <c r="F78" t="s">
+        <v>35</v>
+      </c>
+      <c r="G78" t="s">
+        <v>36</v>
+      </c>
+      <c r="H78" t="s">
+        <v>33</v>
+      </c>
+      <c r="I78" t="s">
+        <v>161</v>
+      </c>
+      <c r="J78" t="s">
+        <v>154</v>
+      </c>
+      <c r="K78" t="s">
+        <v>114</v>
+      </c>
+      <c r="L78" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>135</v>
+      </c>
+      <c r="D79" t="s">
+        <v>131</v>
+      </c>
+      <c r="E79" t="s">
+        <v>34</v>
+      </c>
+      <c r="F79" t="s">
+        <v>30</v>
+      </c>
+      <c r="G79" t="s">
+        <v>33</v>
+      </c>
+      <c r="H79" t="s">
+        <v>28</v>
+      </c>
+      <c r="I79" t="s">
+        <v>42</v>
+      </c>
+      <c r="J79" t="s">
+        <v>9</v>
+      </c>
+      <c r="K79" t="s">
+        <v>212</v>
+      </c>
+      <c r="L79" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C80" t="s">
+        <v>151</v>
+      </c>
+      <c r="D80" t="s">
+        <v>24</v>
+      </c>
+      <c r="E80" t="s">
+        <v>43</v>
+      </c>
+      <c r="F80" t="s">
+        <v>187</v>
+      </c>
+      <c r="G80" t="s">
+        <v>129</v>
+      </c>
+      <c r="H80" t="s">
+        <v>49</v>
+      </c>
+      <c r="I80" t="s">
+        <v>226</v>
+      </c>
+      <c r="J80" t="s">
+        <v>33</v>
+      </c>
+      <c r="K80" t="s">
+        <v>30</v>
+      </c>
+      <c r="L80" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
+        <v>179</v>
+      </c>
+      <c r="D81" t="s">
+        <v>227</v>
+      </c>
+      <c r="E81" t="s">
+        <v>180</v>
+      </c>
+      <c r="F81" t="s">
+        <v>29</v>
+      </c>
+      <c r="G81" t="s">
+        <v>45</v>
+      </c>
+      <c r="H81" t="s">
+        <v>30</v>
+      </c>
+      <c r="I81" t="s">
+        <v>172</v>
+      </c>
+      <c r="J81" t="s">
+        <v>228</v>
+      </c>
+      <c r="K81" t="s">
+        <v>214</v>
+      </c>
+      <c r="L81" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
+        <v>229</v>
+      </c>
+      <c r="D82" t="s">
+        <v>112</v>
+      </c>
+      <c r="E82" t="s">
+        <v>41</v>
+      </c>
+      <c r="F82" t="s">
+        <v>28</v>
+      </c>
+      <c r="G82" t="s">
+        <v>24</v>
+      </c>
+      <c r="H82" t="s">
+        <v>148</v>
+      </c>
+      <c r="I82" t="s">
+        <v>9</v>
+      </c>
+      <c r="J82" t="s">
+        <v>34</v>
+      </c>
+      <c r="K82" t="s">
+        <v>33</v>
+      </c>
+      <c r="L82" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>97</v>
+      </c>
+      <c r="C83" t="s">
+        <v>224</v>
+      </c>
+      <c r="D83" t="s">
+        <v>188</v>
+      </c>
+      <c r="E83" t="s">
+        <v>139</v>
+      </c>
+      <c r="F83" t="s">
+        <v>193</v>
+      </c>
+      <c r="G83" t="s">
+        <v>159</v>
+      </c>
+      <c r="H83" t="s">
+        <v>26</v>
+      </c>
+      <c r="I83" t="s">
+        <v>230</v>
+      </c>
+      <c r="J83" t="s">
+        <v>30</v>
+      </c>
+      <c r="K83" t="s">
+        <v>33</v>
+      </c>
+      <c r="L83" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en los movimientos
</commit_message>
<xml_diff>
--- a/ST/src/principal/Lista de tipos y movimientos de pokémon.xlsx
+++ b/ST/src/principal/Lista de tipos y movimientos de pokémon.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{34424F4C-CD1E-47D1-AFE5-31FDC56CF9BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8920FE56-C46A-48B7-9B5B-B063D1FD6B3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="17360" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17388" windowHeight="13224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="236">
   <si>
     <t>PLANTA</t>
   </si>
@@ -203,9 +203,6 @@
     <t>DRAGONITE</t>
   </si>
   <si>
-    <t>ELEKTROSS</t>
-  </si>
-  <si>
     <t>ESPEON</t>
   </si>
   <si>
@@ -449,12 +446,6 @@
     <t>EVITE IGNEO</t>
   </si>
   <si>
-    <t>PUAS TOXICAS</t>
-  </si>
-  <si>
-    <t>HIDORBOMBA</t>
-  </si>
-  <si>
     <t>DANZA DRAGÓN</t>
   </si>
   <si>
@@ -473,9 +464,6 @@
     <t>PANTALLA LUZ</t>
   </si>
   <si>
-    <t>REFEJO</t>
-  </si>
-  <si>
     <t>HIDROBOMBA</t>
   </si>
   <si>
@@ -509,12 +497,6 @@
     <t>DEMOLICIÓN</t>
   </si>
   <si>
-    <t>AVALNACHA</t>
-  </si>
-  <si>
-    <t>CHUPAVIDAS</t>
-  </si>
-  <si>
     <t>TIJERA X</t>
   </si>
   <si>
@@ -536,9 +518,6 @@
     <t>COME SUEÑOS</t>
   </si>
   <si>
-    <t>PERMONICIÓN</t>
-  </si>
-  <si>
     <t>BOMBA LODO</t>
   </si>
   <si>
@@ -557,9 +536,6 @@
     <t>RESPIRO</t>
   </si>
   <si>
-    <t>ACROBATA</t>
-  </si>
-  <si>
     <t>GIGADRENADO</t>
   </si>
   <si>
@@ -626,9 +602,6 @@
     <t>COLA DRAGON</t>
   </si>
   <si>
-    <t>TERRATEMBLOR</t>
-  </si>
-  <si>
     <t>GARRA UMBRIA</t>
   </si>
   <si>
@@ -659,9 +632,6 @@
     <t>ONDA TÓXICA</t>
   </si>
   <si>
-    <t>PODER OCULTO</t>
-  </si>
-  <si>
     <t>LLUEVE HOJAS</t>
   </si>
   <si>
@@ -683,15 +653,6 @@
     <t>BESO DRENAJE</t>
   </si>
   <si>
-    <t>PAN MENTAL</t>
-  </si>
-  <si>
-    <t>RAPIDEZ</t>
-  </si>
-  <si>
-    <t>HUMREDA</t>
-  </si>
-  <si>
     <t xml:space="preserve">PROTECCIÓN </t>
   </si>
   <si>
@@ -701,19 +662,73 @@
     <t>ESFERA AURAL</t>
   </si>
   <si>
-    <t>ARMADURA ACIDA</t>
-  </si>
-  <si>
-    <t>SOMNIFERO</t>
-  </si>
-  <si>
-    <t>DANZA PETALO</t>
-  </si>
-  <si>
-    <t>CARATOÑA</t>
-  </si>
-  <si>
     <t>ALA DE ACERO</t>
+  </si>
+  <si>
+    <t>HUMAREDA</t>
+  </si>
+  <si>
+    <t>SOMNÍFERO</t>
+  </si>
+  <si>
+    <t>DANZA PÉTALO</t>
+  </si>
+  <si>
+    <t>ÁCROBATA</t>
+  </si>
+  <si>
+    <t>JUEGO SUCIO</t>
+  </si>
+  <si>
+    <t>ARMADURA ÁCIDA</t>
+  </si>
+  <si>
+    <t>MOFA</t>
+  </si>
+  <si>
+    <t>MAQUINACIÓN</t>
+  </si>
+  <si>
+    <t>PÚAS TÓXICAS</t>
+  </si>
+  <si>
+    <t>CARÁMBANO</t>
+  </si>
+  <si>
+    <t>ROMPECORAZA</t>
+  </si>
+  <si>
+    <t>EELEKTROSS</t>
+  </si>
+  <si>
+    <t>DESARME</t>
+  </si>
+  <si>
+    <t>REFLEJO</t>
+  </si>
+  <si>
+    <t>SOL MATINAL</t>
+  </si>
+  <si>
+    <t>PUÑO HIELO</t>
+  </si>
+  <si>
+    <t>RED VISCOSA</t>
+  </si>
+  <si>
+    <t>ZUMBIDO</t>
+  </si>
+  <si>
+    <t>PREMONICIÓN</t>
+  </si>
+  <si>
+    <t>HIERBA LAZO</t>
+  </si>
+  <si>
+    <t>SONÁMBULO</t>
+  </si>
+  <si>
+    <t>ESTALLIDO</t>
   </si>
 </sst>
 </file>
@@ -1033,26 +1048,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.90625" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
-    <col min="5" max="5" width="20.26953125" customWidth="1"/>
-    <col min="6" max="6" width="29.36328125" customWidth="1"/>
-    <col min="7" max="7" width="18.453125" customWidth="1"/>
-    <col min="8" max="8" width="20.26953125" customWidth="1"/>
-    <col min="9" max="9" width="16.1796875" customWidth="1"/>
-    <col min="10" max="10" width="18.90625" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="20.21875" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" customWidth="1"/>
+    <col min="10" max="10" width="18.88671875" customWidth="1"/>
     <col min="11" max="11" width="24" customWidth="1"/>
-    <col min="12" max="12" width="15.81640625" customWidth="1"/>
+    <col min="12" max="12" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>18</v>
       </c>
@@ -1060,7 +1075,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1071,7 +1086,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1082,7 +1097,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1093,7 +1108,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1104,7 +1119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1115,7 +1130,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1126,7 +1141,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1137,7 +1152,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1148,7 +1163,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1159,7 +1174,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1170,7 +1185,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1181,7 +1196,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1192,7 +1207,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1203,7 +1218,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1214,7 +1229,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1225,7 +1240,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1236,7 +1251,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1247,7 +1262,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1258,74 +1273,74 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L32">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>50</v>
       </c>
       <c r="C33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" t="s">
         <v>98</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>99</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>100</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>101</v>
-      </c>
-      <c r="G33" t="s">
-        <v>102</v>
       </c>
       <c r="H33" t="s">
         <v>43</v>
@@ -1343,42 +1358,42 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>51</v>
       </c>
       <c r="C34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" t="s">
         <v>103</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>104</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>105</v>
-      </c>
-      <c r="F34" t="s">
-        <v>106</v>
       </c>
       <c r="G34" t="s">
         <v>28</v>
       </c>
       <c r="H34" t="s">
+        <v>106</v>
+      </c>
+      <c r="I34" t="s">
         <v>107</v>
-      </c>
-      <c r="I34" t="s">
-        <v>108</v>
       </c>
       <c r="J34" t="s">
         <v>40</v>
       </c>
       <c r="K34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L34" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1386,34 +1401,34 @@
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F35" t="s">
+        <v>111</v>
+      </c>
+      <c r="G35" t="s">
+        <v>110</v>
+      </c>
+      <c r="H35" t="s">
+        <v>107</v>
+      </c>
+      <c r="I35" t="s">
         <v>112</v>
-      </c>
-      <c r="G35" t="s">
-        <v>111</v>
-      </c>
-      <c r="H35" t="s">
-        <v>108</v>
-      </c>
-      <c r="I35" t="s">
-        <v>113</v>
       </c>
       <c r="J35" t="s">
         <v>45</v>
       </c>
       <c r="K35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1430,7 +1445,7 @@
         <v>43</v>
       </c>
       <c r="G36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H36" t="s">
         <v>30</v>
@@ -1442,103 +1457,103 @@
         <v>26</v>
       </c>
       <c r="K36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>53</v>
       </c>
       <c r="C37" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" t="s">
         <v>116</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>117</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>118</v>
       </c>
-      <c r="F37" t="s">
-        <v>119</v>
-      </c>
       <c r="G37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I37" t="s">
         <v>36</v>
       </c>
       <c r="J37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K37" t="s">
+        <v>119</v>
+      </c>
+      <c r="L37" t="s">
         <v>120</v>
       </c>
-      <c r="L37" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>54</v>
       </c>
       <c r="C38" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" t="s">
         <v>122</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>123</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>124</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>125</v>
-      </c>
-      <c r="G38" t="s">
-        <v>126</v>
       </c>
       <c r="H38" t="s">
         <v>35</v>
       </c>
       <c r="I38" t="s">
+        <v>126</v>
+      </c>
+      <c r="J38" t="s">
+        <v>120</v>
+      </c>
+      <c r="K38" t="s">
         <v>127</v>
       </c>
-      <c r="J38" t="s">
-        <v>121</v>
-      </c>
-      <c r="K38" t="s">
-        <v>128</v>
-      </c>
       <c r="L38" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>55</v>
       </c>
       <c r="C39" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" t="s">
         <v>129</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>130</v>
       </c>
-      <c r="E39" t="s">
-        <v>131</v>
-      </c>
       <c r="F39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G39" t="s">
         <v>26</v>
       </c>
       <c r="H39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I39" t="s">
         <v>30</v>
@@ -1550,21 +1565,21 @@
         <v>28</v>
       </c>
       <c r="L39" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>56</v>
       </c>
       <c r="C40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D40" t="s">
         <v>30</v>
       </c>
       <c r="E40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F40" t="s">
         <v>28</v>
@@ -1573,65 +1588,65 @@
         <v>26</v>
       </c>
       <c r="H40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I40" t="s">
+        <v>134</v>
+      </c>
+      <c r="J40" t="s">
+        <v>33</v>
+      </c>
+      <c r="K40" t="s">
         <v>135</v>
-      </c>
-      <c r="J40" t="s">
-        <v>33</v>
-      </c>
-      <c r="K40" t="s">
-        <v>136</v>
       </c>
       <c r="L40" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>57</v>
       </c>
       <c r="C41" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" t="s">
         <v>137</v>
       </c>
-      <c r="D41" t="s">
-        <v>138</v>
-      </c>
       <c r="E41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F41" t="s">
         <v>36</v>
       </c>
       <c r="G41" t="s">
+        <v>138</v>
+      </c>
+      <c r="H41" t="s">
+        <v>33</v>
+      </c>
+      <c r="I41" t="s">
+        <v>121</v>
+      </c>
+      <c r="J41" t="s">
         <v>139</v>
       </c>
-      <c r="H41" t="s">
-        <v>33</v>
-      </c>
-      <c r="I41" t="s">
-        <v>122</v>
-      </c>
-      <c r="J41" t="s">
+      <c r="K41" t="s">
+        <v>120</v>
+      </c>
+      <c r="L41" t="s">
         <v>140</v>
       </c>
-      <c r="K41" t="s">
-        <v>121</v>
-      </c>
-      <c r="L41" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>58</v>
       </c>
       <c r="C42" t="s">
-        <v>142</v>
+        <v>222</v>
       </c>
       <c r="D42" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="E42" t="s">
         <v>24</v>
@@ -1649,33 +1664,33 @@
         <v>30</v>
       </c>
       <c r="J42" t="s">
-        <v>42</v>
+        <v>223</v>
       </c>
       <c r="K42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>59</v>
       </c>
       <c r="C43" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F43" t="s">
         <v>41</v>
       </c>
       <c r="G43" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H43" t="s">
         <v>37</v>
@@ -1693,18 +1708,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
       <c r="C44" t="s">
-        <v>44</v>
+        <v>226</v>
       </c>
       <c r="D44" t="s">
-        <v>146</v>
+        <v>23</v>
       </c>
       <c r="E44" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="F44" t="s">
         <v>30</v>
@@ -1722,21 +1737,21 @@
         <v>33</v>
       </c>
       <c r="K44" t="s">
-        <v>147</v>
+        <v>31</v>
       </c>
       <c r="L44" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C45" t="s">
         <v>28</v>
       </c>
       <c r="D45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E45" t="s">
         <v>33</v>
@@ -1748,30 +1763,30 @@
         <v>26</v>
       </c>
       <c r="H45" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I45" t="s">
-        <v>150</v>
+        <v>227</v>
       </c>
       <c r="J45" t="s">
         <v>42</v>
       </c>
       <c r="K45" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L45" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D46" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E46" t="s">
         <v>44</v>
@@ -1786,24 +1801,24 @@
         <v>24</v>
       </c>
       <c r="I46" t="s">
-        <v>43</v>
+        <v>229</v>
       </c>
       <c r="J46" t="s">
         <v>42</v>
       </c>
       <c r="K46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L46" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D47" t="s">
         <v>45</v>
@@ -1815,13 +1830,13 @@
         <v>30</v>
       </c>
       <c r="G47" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H47" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="I47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J47" t="s">
         <v>42</v>
@@ -1833,9 +1848,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48" t="s">
         <v>24</v>
@@ -1844,10 +1859,10 @@
         <v>43</v>
       </c>
       <c r="E48" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G48" t="s">
         <v>28</v>
@@ -1865,27 +1880,27 @@
         <v>33</v>
       </c>
       <c r="L48" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D49" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E49" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F49" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H49" t="s">
         <v>33</v>
@@ -1894,18 +1909,18 @@
         <v>9</v>
       </c>
       <c r="J49" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K49" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="L49" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
         <v>47</v>
@@ -1914,13 +1929,13 @@
         <v>41</v>
       </c>
       <c r="E50" t="s">
-        <v>139</v>
+        <v>23</v>
       </c>
       <c r="F50" t="s">
-        <v>163</v>
+        <v>231</v>
       </c>
       <c r="G50" t="s">
-        <v>164</v>
+        <v>230</v>
       </c>
       <c r="H50" t="s">
         <v>33</v>
@@ -1932,18 +1947,18 @@
         <v>29</v>
       </c>
       <c r="K50" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="L50" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D51" t="s">
         <v>45</v>
@@ -1952,45 +1967,45 @@
         <v>44</v>
       </c>
       <c r="F51" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G51" t="s">
         <v>46</v>
       </c>
       <c r="H51" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="I51" t="s">
         <v>30</v>
       </c>
       <c r="J51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K51" t="s">
         <v>35</v>
       </c>
       <c r="L51" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C52" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E52" t="s">
         <v>26</v>
       </c>
       <c r="F52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G52" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="H52" t="s">
         <v>33</v>
@@ -2002,68 +2017,68 @@
         <v>28</v>
       </c>
       <c r="K52" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="L52" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C53" t="s">
         <v>28</v>
       </c>
       <c r="D53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F53" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G53" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H53" t="s">
         <v>33</v>
       </c>
       <c r="I53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J53" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K53" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="L53" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C54" t="s">
         <v>24</v>
       </c>
       <c r="D54" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F54" t="s">
         <v>43</v>
       </c>
       <c r="G54" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="H54" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="I54" t="s">
         <v>33</v>
@@ -2075,27 +2090,27 @@
         <v>30</v>
       </c>
       <c r="L54" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C55" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D55" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G55" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="H55" t="s">
         <v>33</v>
@@ -2107,24 +2122,24 @@
         <v>35</v>
       </c>
       <c r="K55" t="s">
-        <v>178</v>
+        <v>217</v>
       </c>
       <c r="L55" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E56" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F56" t="s">
         <v>30</v>
@@ -2136,10 +2151,10 @@
         <v>33</v>
       </c>
       <c r="I56" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J56" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="K56" t="s">
         <v>29</v>
@@ -2148,9 +2163,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C57" t="s">
         <v>47</v>
@@ -2168,36 +2183,36 @@
         <v>28</v>
       </c>
       <c r="H57" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="I57" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="J57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K57" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="L57" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C58" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E58" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F58" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="G58" t="s">
         <v>30</v>
@@ -2215,30 +2230,30 @@
         <v>45</v>
       </c>
       <c r="L58" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C59" t="s">
         <v>49</v>
       </c>
       <c r="D59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E59" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F59" t="s">
         <v>24</v>
       </c>
       <c r="G59" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="H59" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="I59" t="s">
         <v>42</v>
@@ -2250,18 +2265,18 @@
         <v>30</v>
       </c>
       <c r="L59" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s">
         <v>47</v>
       </c>
       <c r="D60" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E60" t="s">
         <v>44</v>
@@ -2276,36 +2291,36 @@
         <v>33</v>
       </c>
       <c r="I60" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J60" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K60" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="L60" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C61" t="s">
         <v>35</v>
       </c>
       <c r="D61" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E61" t="s">
         <v>46</v>
       </c>
       <c r="F61" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="G61" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H61" t="s">
         <v>30</v>
@@ -2314,18 +2329,18 @@
         <v>33</v>
       </c>
       <c r="J61" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L61" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C62" t="s">
         <v>47</v>
@@ -2337,10 +2352,10 @@
         <v>41</v>
       </c>
       <c r="F62" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="G62" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="H62" t="s">
         <v>30</v>
@@ -2349,30 +2364,30 @@
         <v>33</v>
       </c>
       <c r="J62" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K62" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="L62" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C63" t="s">
-        <v>9</v>
+        <v>233</v>
       </c>
       <c r="D63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E63" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F63" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="G63" t="s">
         <v>45</v>
@@ -2381,21 +2396,21 @@
         <v>46</v>
       </c>
       <c r="I63" t="s">
-        <v>172</v>
+        <v>103</v>
       </c>
       <c r="J63" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="K63" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="L63" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C64" t="s">
         <v>49</v>
@@ -2404,13 +2419,13 @@
         <v>24</v>
       </c>
       <c r="E64" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F64" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G64" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="H64" t="s">
         <v>43</v>
@@ -2419,36 +2434,36 @@
         <v>30</v>
       </c>
       <c r="J64" t="s">
-        <v>201</v>
+        <v>34</v>
       </c>
       <c r="K64" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L64" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C65" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D65" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F65" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G65" t="s">
         <v>28</v>
       </c>
       <c r="H65" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I65" t="s">
         <v>9</v>
@@ -2457,27 +2472,27 @@
         <v>33</v>
       </c>
       <c r="K65" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="L65" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D66" t="s">
         <v>26</v>
       </c>
       <c r="E66" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F66" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G66" t="s">
         <v>41</v>
@@ -2486,7 +2501,7 @@
         <v>28</v>
       </c>
       <c r="I66" t="s">
-        <v>204</v>
+        <v>23</v>
       </c>
       <c r="J66" t="s">
         <v>29</v>
@@ -2495,47 +2510,47 @@
         <v>30</v>
       </c>
       <c r="L66" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C67" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="D67" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E67" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F67" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="G67" t="s">
         <v>41</v>
       </c>
       <c r="H67" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="I67" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="J67" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="K67" t="s">
         <v>30</v>
       </c>
       <c r="L67" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C68" t="s">
         <v>9</v>
@@ -2544,16 +2559,16 @@
         <v>23</v>
       </c>
       <c r="E68" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F68" t="s">
         <v>33</v>
       </c>
       <c r="G68" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H68" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="I68" t="s">
         <v>47</v>
@@ -2562,21 +2577,21 @@
         <v>30</v>
       </c>
       <c r="K68" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="L68" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C69" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D69" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E69" t="s">
         <v>28</v>
@@ -2585,10 +2600,10 @@
         <v>29</v>
       </c>
       <c r="G69" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="H69" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="I69" t="s">
         <v>33</v>
@@ -2597,30 +2612,30 @@
         <v>9</v>
       </c>
       <c r="K69" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="L69" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C70" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D70" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E70" t="s">
         <v>30</v>
       </c>
       <c r="F70" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="G70" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H70" t="s">
         <v>31</v>
@@ -2629,33 +2644,33 @@
         <v>33</v>
       </c>
       <c r="J70" t="s">
-        <v>189</v>
+        <v>220</v>
       </c>
       <c r="K70" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="L70" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C71" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E71" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F71" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="G71" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H71" t="s">
         <v>36</v>
@@ -2664,7 +2679,7 @@
         <v>45</v>
       </c>
       <c r="J71" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K71" t="s">
         <v>30</v>
@@ -2673,30 +2688,30 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>21</v>
       </c>
       <c r="C72" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="D72" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E72" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F72" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G72" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="H72" t="s">
         <v>30</v>
       </c>
       <c r="I72" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="J72" t="s">
         <v>45</v>
@@ -2705,123 +2720,123 @@
         <v>33</v>
       </c>
       <c r="L72" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C73" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D73" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E73" t="s">
         <v>29</v>
       </c>
       <c r="F73" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="G73" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="H73" t="s">
         <v>30</v>
       </c>
       <c r="I73" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="J73" t="s">
         <v>33</v>
       </c>
       <c r="K73" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="L73" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
       </c>
       <c r="D74" t="s">
+        <v>130</v>
+      </c>
+      <c r="E74" t="s">
+        <v>102</v>
+      </c>
+      <c r="F74" t="s">
+        <v>208</v>
+      </c>
+      <c r="G74" t="s">
+        <v>134</v>
+      </c>
+      <c r="H74" t="s">
         <v>131</v>
       </c>
-      <c r="E74" t="s">
-        <v>103</v>
-      </c>
-      <c r="F74" t="s">
-        <v>218</v>
-      </c>
-      <c r="G74" t="s">
-        <v>135</v>
-      </c>
-      <c r="H74" t="s">
-        <v>132</v>
-      </c>
       <c r="I74" t="s">
         <v>30</v>
       </c>
       <c r="J74" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="K74" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="L74" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C75" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D75" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="E75" t="s">
-        <v>220</v>
+        <v>131</v>
       </c>
       <c r="F75" t="s">
         <v>28</v>
       </c>
       <c r="G75" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="H75" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="I75" t="s">
         <v>30</v>
       </c>
       <c r="J75" t="s">
-        <v>221</v>
+        <v>28</v>
       </c>
       <c r="K75" t="s">
         <v>33</v>
       </c>
       <c r="L75" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C76" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="D76" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="E76" t="s">
         <v>26</v>
@@ -2830,60 +2845,60 @@
         <v>28</v>
       </c>
       <c r="G76" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="H76" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="I76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J76" t="s">
         <v>41</v>
       </c>
       <c r="K76" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="L76" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C77" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D77" t="s">
         <v>45</v>
       </c>
       <c r="E77" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F77" t="s">
-        <v>112</v>
+        <v>48</v>
       </c>
       <c r="G77" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H77" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I77" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="J77" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K77" t="s">
         <v>34</v>
       </c>
       <c r="L77" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>20</v>
       </c>
@@ -2894,7 +2909,7 @@
         <v>45</v>
       </c>
       <c r="E78" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F78" t="s">
         <v>35</v>
@@ -2906,27 +2921,27 @@
         <v>33</v>
       </c>
       <c r="I78" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J78" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L78" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C79" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D79" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E79" t="s">
         <v>34</v>
@@ -2947,18 +2962,18 @@
         <v>9</v>
       </c>
       <c r="K79" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="L79" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C80" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D80" t="s">
         <v>24</v>
@@ -2967,16 +2982,16 @@
         <v>43</v>
       </c>
       <c r="F80" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="G80" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H80" t="s">
-        <v>49</v>
+        <v>219</v>
       </c>
       <c r="I80" t="s">
-        <v>226</v>
+        <v>163</v>
       </c>
       <c r="J80" t="s">
         <v>33</v>
@@ -2988,18 +3003,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C81" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D81" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="E81" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F81" t="s">
         <v>29</v>
@@ -3011,27 +3026,27 @@
         <v>30</v>
       </c>
       <c r="I81" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="J81" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="K81" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="L81" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C82" t="s">
-        <v>229</v>
+        <v>39</v>
       </c>
       <c r="D82" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E82" t="s">
         <v>41</v>
@@ -3043,10 +3058,10 @@
         <v>24</v>
       </c>
       <c r="H82" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I82" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="J82" t="s">
         <v>34</v>
@@ -3058,30 +3073,30 @@
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C83" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="D83" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="E83" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F83" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="G83" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H83" t="s">
         <v>26</v>
       </c>
       <c r="I83" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="J83" t="s">
         <v>30</v>
@@ -3090,7 +3105,7 @@
         <v>33</v>
       </c>
       <c r="L83" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>